<commit_message>
Add updated parameter in Upload Bucket, MessageGroupId
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_UploadBucket/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_UploadBucket/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_UploadBucket\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Kalyana\Traveloka_DataAutomation_UploadBucket\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7585BD8A-CE06-4CE9-BE21-9A6C2C0A8FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DF6F34-0764-4F4A-9AB9-4749532EFC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,15 @@
     <t>AWS_BucketName</t>
   </si>
   <si>
+    <t>RPA_Moon_AWS_BucketName</t>
+  </si>
+  <si>
     <t>AWS_IAMRole</t>
   </si>
   <si>
+    <t>RPA_Moon_AWS_IAMRole</t>
+  </si>
+  <si>
     <t>AWS_Region</t>
   </si>
   <si>
@@ -186,22 +192,16 @@
     <t>AWS_SQS_QueueName</t>
   </si>
   <si>
-    <t>[DEV] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
-    <t>[DEV] RPA_Moon_AWS_BucketName</t>
-  </si>
-  <si>
-    <t>[DEV] RPA_Moon_AWS_IAMRole</t>
-  </si>
-  <si>
-    <t>[DEV] RPA_Moon_AWS_SQS_QueueName</t>
+    <t>RPA_Moon_AWS_SQS_QueueName</t>
+  </si>
+  <si>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>EmailSenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
-  </si>
-  <si>
-    <t>EmailSenderName</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -630,7 +630,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2834,7 +2834,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2886,23 +2886,23 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2910,23 +2910,23 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>